<commit_message>
upgrade: adding a color to graph
</commit_message>
<xml_diff>
--- a/VALE3.SA.xlsx
+++ b/VALE3.SA.xlsx
@@ -585,7 +585,7 @@
         <v>9509400</v>
       </c>
       <c r="H2">
-        <v>18.71414566040039</v>
+        <v>18.89414596557617</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
@@ -10741,25 +10741,25 @@
         <v>61.93999862670898</v>
       </c>
       <c r="D250">
-        <v>61.29000091552734</v>
+        <v>60.84999847412109</v>
       </c>
       <c r="E250">
-        <v>61.41999816894531</v>
+        <v>61.59999847412109</v>
       </c>
       <c r="F250">
-        <v>61.41999816894531</v>
+        <v>61.59999847412109</v>
       </c>
       <c r="G250">
-        <v>2517000</v>
+        <v>21120900</v>
       </c>
       <c r="H250">
-        <v>-0.1299972534179688</v>
+        <v>-0.30999755859375</v>
       </c>
       <c r="I250" t="s">
         <v>14</v>
       </c>
       <c r="J250">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K250" t="s">
         <v>15</v>

</xml_diff>